<commit_message>
merge and setup for alpha
</commit_message>
<xml_diff>
--- a/RapZapSnap/Assets/Chew/script/Excel Related/NotesData2.xlsx
+++ b/RapZapSnap/Assets/Chew/script/Excel Related/NotesData2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-45" windowWidth="12630" windowHeight="5445" activeTab="2"/>
+    <workbookView xWindow="-60" yWindow="-45" windowWidth="12630" windowHeight="5445" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Phrase1" sheetId="1" r:id="rId1"/>
@@ -930,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -1358,6 +1358,9 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>17</v>
+      </c>
       <c r="B18">
         <v>11</v>
       </c>
@@ -1381,6 +1384,9 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>18</v>
+      </c>
       <c r="B19">
         <v>-11</v>
       </c>
@@ -1418,8 +1424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -1846,6 +1852,9 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>17</v>
+      </c>
       <c r="B18">
         <v>11</v>
       </c>
@@ -1869,6 +1878,9 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>18</v>
+      </c>
       <c r="B19">
         <v>3.55</v>
       </c>

</xml_diff>